<commit_message>
add some calcul methods
</commit_message>
<xml_diff>
--- a/platform_inputs/input_S3.xlsx
+++ b/platform_inputs/input_S3.xlsx
@@ -1010,10 +1010,10 @@
       </c>
       <c r="H5" s="14" t="n"/>
       <c r="I5" s="17" t="n">
-        <v>29475</v>
+        <v>13467</v>
       </c>
       <c r="J5" s="18" t="n">
-        <v>17777</v>
+        <v>16509</v>
       </c>
       <c r="K5" s="17" t="n">
         <v>29475</v>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="H7" s="23" t="n"/>
       <c r="I7" s="24" t="n">
-        <v>21822</v>
+        <v>5508</v>
       </c>
       <c r="J7" s="24" t="n">
         <v>4492</v>
@@ -1212,19 +1212,19 @@
         <v>5068</v>
       </c>
       <c r="Q7" s="24" t="n">
+        <v>9961</v>
+      </c>
+      <c r="R7" s="24" t="n">
+        <v>9682</v>
+      </c>
+      <c r="S7" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="R7" s="24" t="n">
-        <v>19643</v>
-      </c>
-      <c r="S7" s="24" t="n">
-        <v>9213</v>
-      </c>
       <c r="T7" s="24" t="n">
-        <v>5759</v>
+        <v>5075</v>
       </c>
       <c r="U7" s="24" t="n">
-        <v>5447</v>
+        <v>15344</v>
       </c>
       <c r="V7" s="24" t="n">
         <v>5104</v>
@@ -1257,7 +1257,7 @@
         <v>8967</v>
       </c>
       <c r="AF7" s="24" t="n">
-        <v>12621</v>
+        <v>3979</v>
       </c>
       <c r="AG7" s="24" t="n"/>
       <c r="AH7" s="24" t="n"/>
@@ -1478,7 +1478,7 @@
         <v>678</v>
       </c>
       <c r="AE9" s="27" t="n">
-        <v>7027</v>
+        <v>7155</v>
       </c>
       <c r="AF9" s="27" t="n">
         <v>0</v>
@@ -1639,10 +1639,10 @@
         <v>3543</v>
       </c>
       <c r="J11" s="27" t="n">
-        <v>10046</v>
+        <v>6477</v>
       </c>
       <c r="K11" s="27" t="n">
-        <v>4133</v>
+        <v>7702</v>
       </c>
       <c r="L11" s="27" t="n">
         <v>1387</v>
@@ -1651,31 +1651,31 @@
         <v>3758</v>
       </c>
       <c r="N11" s="27" t="n">
-        <v>5205</v>
+        <v>17557</v>
       </c>
       <c r="O11" s="27" t="n">
-        <v>5902</v>
+        <v>26499</v>
       </c>
       <c r="P11" s="27" t="n">
-        <v>3347</v>
+        <v>0</v>
       </c>
       <c r="Q11" s="27" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="R11" s="27" t="n">
-        <v>7474</v>
+        <v>0</v>
       </c>
       <c r="S11" s="27" t="n">
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="T11" s="27" t="n">
-        <v>5558</v>
+        <v>0</v>
       </c>
       <c r="U11" s="27" t="n">
-        <v>6316</v>
+        <v>0</v>
       </c>
       <c r="V11" s="27" t="n">
-        <v>7606</v>
+        <v>4848</v>
       </c>
       <c r="W11" s="27" t="n">
         <v>4824</v>
@@ -1699,7 +1699,7 @@
         <v>7386</v>
       </c>
       <c r="AD11" s="27" t="n">
-        <v>4902</v>
+        <v>4899</v>
       </c>
       <c r="AE11" s="27" t="n">
         <v>0</v>
@@ -1920,7 +1920,7 @@
         <v>13794</v>
       </c>
       <c r="AC13" s="27" t="n">
-        <v>13542</v>
+        <v>14998</v>
       </c>
       <c r="AD13" s="27" t="n">
         <v>0</v>
@@ -2120,10 +2120,10 @@
       </c>
       <c r="H16" s="14" t="n"/>
       <c r="I16" s="17" t="n">
-        <v>27900</v>
+        <v>30299</v>
       </c>
       <c r="J16" s="18" t="n">
-        <v>5830</v>
+        <v>14814</v>
       </c>
       <c r="K16" s="17" t="n">
         <v>27900</v>
@@ -2298,16 +2298,16 @@
       </c>
       <c r="H18" s="23" t="n"/>
       <c r="I18" s="24" t="n">
-        <v>20633</v>
+        <v>7025</v>
       </c>
       <c r="J18" s="24" t="n">
         <v>2975</v>
       </c>
       <c r="K18" s="24" t="n">
-        <v>4920</v>
+        <v>4822</v>
       </c>
       <c r="L18" s="24" t="n">
-        <v>3750</v>
+        <v>3848</v>
       </c>
       <c r="M18" s="25" t="n">
         <v>9196</v>
@@ -2328,10 +2328,10 @@
         <v>3551</v>
       </c>
       <c r="S18" s="24" t="n">
-        <v>5116</v>
+        <v>6800</v>
       </c>
       <c r="T18" s="24" t="n">
-        <v>3520</v>
+        <v>1836</v>
       </c>
       <c r="U18" s="24" t="n">
         <v>7201</v>
@@ -2367,7 +2367,7 @@
         <v>3086</v>
       </c>
       <c r="AF18" s="24" t="n">
-        <v>2817</v>
+        <v>12890</v>
       </c>
       <c r="AG18" s="24" t="n"/>
       <c r="AH18" s="24" t="n"/>
@@ -2588,7 +2588,7 @@
         <v>333</v>
       </c>
       <c r="AE20" s="27" t="n">
-        <v>5056</v>
+        <v>735</v>
       </c>
       <c r="AF20" s="27" t="n">
         <v>0</v>
@@ -2806,7 +2806,7 @@
         <v>14187</v>
       </c>
       <c r="AC22" s="27" t="n">
-        <v>7024</v>
+        <v>1462</v>
       </c>
       <c r="AD22" s="27" t="n">
         <v>0</v>
@@ -3006,10 +3006,10 @@
       </c>
       <c r="H25" s="14" t="n"/>
       <c r="I25" s="17" t="n">
-        <v>8262</v>
+        <v>8906</v>
       </c>
       <c r="J25" s="18" t="n">
-        <v>13291</v>
+        <v>14811</v>
       </c>
       <c r="K25" s="17" t="n">
         <v>8262</v>
@@ -3184,16 +3184,16 @@
       </c>
       <c r="H27" s="23" t="n"/>
       <c r="I27" s="24" t="n">
-        <v>17237</v>
+        <v>435</v>
       </c>
       <c r="J27" s="24" t="n">
         <v>9565</v>
       </c>
       <c r="K27" s="24" t="n">
-        <v>2478</v>
+        <v>1635</v>
       </c>
       <c r="L27" s="24" t="n">
-        <v>7919</v>
+        <v>8762</v>
       </c>
       <c r="M27" s="25" t="n">
         <v>699</v>
@@ -3253,7 +3253,7 @@
         <v>2976</v>
       </c>
       <c r="AF27" s="24" t="n">
-        <v>6005</v>
+        <v>8978</v>
       </c>
       <c r="AG27" s="24" t="n"/>
       <c r="AH27" s="24" t="n"/>
@@ -3417,25 +3417,25 @@
         <v>5784</v>
       </c>
       <c r="L29" s="27" t="n">
-        <v>5372</v>
+        <v>11552</v>
       </c>
       <c r="M29" s="27" t="n">
-        <v>8835</v>
+        <v>2655</v>
       </c>
       <c r="N29" s="27" t="n">
-        <v>409</v>
+        <v>25830</v>
       </c>
       <c r="O29" s="27" t="n">
-        <v>5712</v>
+        <v>0</v>
       </c>
       <c r="P29" s="27" t="n">
-        <v>8359</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="27" t="n">
-        <v>4713</v>
+        <v>0</v>
       </c>
       <c r="R29" s="27" t="n">
-        <v>7954</v>
+        <v>1317</v>
       </c>
       <c r="S29" s="27" t="n">
         <v>3226</v>
@@ -3471,7 +3471,7 @@
         <v>4988</v>
       </c>
       <c r="AD29" s="27" t="n">
-        <v>404</v>
+        <v>4723</v>
       </c>
       <c r="AE29" s="27" t="n">
         <v>0</v>
@@ -3668,10 +3668,10 @@
       </c>
       <c r="H32" s="14" t="n"/>
       <c r="I32" s="17" t="n">
-        <v>7673</v>
+        <v>4616</v>
       </c>
       <c r="J32" s="18" t="n">
-        <v>2807</v>
+        <v>4141</v>
       </c>
       <c r="K32" s="17" t="n">
         <v>7673</v>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="H34" s="23" t="n"/>
       <c r="I34" s="24" t="n">
-        <v>16303</v>
+        <v>6822</v>
       </c>
       <c r="J34" s="24" t="n">
         <v>3178</v>
@@ -3879,10 +3879,10 @@
         <v>7944</v>
       </c>
       <c r="T34" s="24" t="n">
-        <v>1091</v>
+        <v>9485</v>
       </c>
       <c r="U34" s="24" t="n">
-        <v>9011</v>
+        <v>617</v>
       </c>
       <c r="V34" s="24" t="n">
         <v>2895</v>
@@ -3915,7 +3915,7 @@
         <v>715</v>
       </c>
       <c r="AF34" s="24" t="n">
-        <v>2935</v>
+        <v>6551</v>
       </c>
       <c r="AG34" s="24" t="n"/>
       <c r="AH34" s="24" t="n"/>

</xml_diff>